<commit_message>
Commit - 21Aprl2023 - 4:05pm
</commit_message>
<xml_diff>
--- a/Hackathon/src/test/resources/ExcelFiles/IngredientsAndComorbidities-ScrapperHackathon.xlsx
+++ b/Hackathon/src/test/resources/ExcelFiles/IngredientsAndComorbidities-ScrapperHackathon.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NumpyNinja_Projects\Hackathon\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRepository\Hackathon\src\test\resources\ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2912A3AB-FA3D-4177-B6B3-89A81AEA0C07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{986CB1C7-8445-4C66-880B-B3E584FCD9E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="199">
   <si>
     <t>Diabetes</t>
   </si>
@@ -614,6 +614,9 @@
   </si>
   <si>
     <t>coriander</t>
+  </si>
+  <si>
+    <t>turmeric</t>
   </si>
 </sst>
 </file>
@@ -2084,8 +2087,8 @@
   </sheetPr>
   <dimension ref="A1:X1002"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -3118,7 +3121,9 @@
       <c r="A27" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="B27" s="13"/>
+      <c r="B27" s="13" t="s">
+        <v>198</v>
+      </c>
       <c r="C27" s="9" t="s">
         <v>74</v>
       </c>

</xml_diff>